<commit_message>
new google and amazon
</commit_message>
<xml_diff>
--- a/amazon-summary.xlsx
+++ b/amazon-summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/narijohnson/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/narijohnson/Documents/CS105-Speech-Algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511359B1-F7A7-6B44-BE8D-8FA496325CAE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D26DAE-5399-3A46-95A3-589B562C43AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19260" yWindow="460" windowWidth="11520" windowHeight="15940" xr2:uid="{A553F17A-A65B-B844-9CF8-B6E8C465C73E}"/>
+    <workbookView xWindow="17280" yWindow="460" windowWidth="11520" windowHeight="15940" xr2:uid="{A553F17A-A65B-B844-9CF8-B6E8C465C73E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Category</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>UKEnglish</t>
+  </si>
+  <si>
+    <t>USEnglish</t>
   </si>
 </sst>
 </file>
@@ -438,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C7DD76-D045-4345-B904-E89F29C83AB3}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,6 +711,40 @@
         <v>10.3</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>21.37</v>
+      </c>
+      <c r="C17">
+        <v>12.9</v>
+      </c>
+      <c r="D17">
+        <v>6.125</v>
+      </c>
+      <c r="E17">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="C18">
+        <v>23</v>
+      </c>
+      <c r="D18">
+        <v>10.9</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>